<commit_message>
switch to data table instead of traditional shiny widgets
change to data table layout for visual compactness and easy of changing
parameters
</commit_message>
<xml_diff>
--- a/nitrogen_cycle_dynamics/nox_isotope_dynamics.xlsx
+++ b/nitrogen_cycle_dynamics/nox_isotope_dynamics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="0" windowWidth="29420" windowHeight="18300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="22580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="168">
   <si>
     <t>id</t>
   </si>
@@ -567,6 +567,21 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>flux</t>
+  </si>
+  <si>
+    <t>mass_flux</t>
+  </si>
+  <si>
+    <t>Mass flux</t>
+  </si>
+  <si>
+    <t>meq/L</t>
+  </si>
+  <si>
+    <t>\\Delta\\left[S\\right]</t>
   </si>
 </sst>
 </file>
@@ -634,7 +649,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -701,6 +716,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -813,7 +832,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -906,6 +925,8 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -980,6 +1001,8 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1309,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1363,135 +1386,141 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>165</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="I2" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>42</v>
       </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="G3" s="3">
-        <v>0.8</v>
+        <v>5</v>
       </c>
       <c r="H3" s="3">
-        <v>1.2</v>
+        <v>30</v>
       </c>
       <c r="I3" s="3">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>42</v>
       </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3">
-        <v>25</v>
+        <v>0.8</v>
       </c>
       <c r="H4" s="3">
-        <v>30</v>
+        <v>1.2</v>
       </c>
       <c r="I4" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>42</v>
       </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="3">
-        <v>-9.1</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3">
-        <v>-20.6</v>
+        <v>30</v>
       </c>
       <c r="I5" s="3">
-        <v>-13</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>42</v>
       </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>91</v>
@@ -1500,16 +1529,16 @@
         <v>8</v>
       </c>
       <c r="G6" s="3">
-        <v>-1.3</v>
+        <v>-9.1</v>
       </c>
       <c r="H6" s="3">
-        <v>-8.1999999999999993</v>
+        <v>-20.6</v>
       </c>
       <c r="I6" s="3">
-        <v>-5</v>
+        <v>-13</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K6" t="s">
         <v>93</v>
@@ -1519,29 +1548,32 @@
       <c r="A7" t="s">
         <v>42</v>
       </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="3">
-        <v>12.8</v>
+        <v>-1.3</v>
       </c>
       <c r="H7" s="3">
-        <v>18.2</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="I7" s="3">
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="J7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K7" t="s">
         <v>93</v>
@@ -1551,552 +1583,585 @@
       <c r="A8" t="s">
         <v>42</v>
       </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="3">
-        <v>5</v>
+        <v>12.8</v>
       </c>
       <c r="H8" s="3">
-        <v>25</v>
+        <v>18.2</v>
       </c>
       <c r="I8" s="3">
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>98</v>
+      </c>
+      <c r="K8" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>42</v>
       </c>
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="3">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="I9" s="3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>42</v>
       </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="3">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="I10" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>42</v>
       </c>
+      <c r="B11" t="s">
+        <v>162</v>
+      </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="G11" s="3">
-        <v>0.01</v>
+        <v>18</v>
       </c>
       <c r="H11" s="3">
-        <v>0.25</v>
+        <v>38</v>
       </c>
       <c r="I11" s="3">
-        <v>0.2</v>
+        <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>42</v>
       </c>
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="G12" s="3">
-        <v>5</v>
+        <v>0.01</v>
       </c>
       <c r="H12" s="3">
-        <v>17</v>
+        <v>0.25</v>
       </c>
       <c r="I12" s="3">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>42</v>
       </c>
+      <c r="B13" t="s">
+        <v>162</v>
+      </c>
       <c r="C13" t="s">
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="3">
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I13" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="K13" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>42</v>
       </c>
+      <c r="B14" t="s">
+        <v>162</v>
+      </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="3">
-        <v>14</v>
+        <v>-2</v>
       </c>
       <c r="H14" s="3">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="I14" s="3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>66</v>
+      </c>
+      <c r="K14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>42</v>
       </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G15" s="3">
+        <v>14</v>
+      </c>
+      <c r="H15" s="3">
+        <v>27</v>
+      </c>
       <c r="I15" s="3">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>88</v>
-      </c>
-      <c r="K15" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="I16" s="3">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>135</v>
+        <v>88</v>
+      </c>
+      <c r="K16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>43</v>
       </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
       </c>
       <c r="H17" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I17" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B18" t="s">
-        <v>162</v>
-      </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
       </c>
       <c r="I18" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>29</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>162</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I19" s="3">
+        <v>6</v>
+      </c>
       <c r="J19" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="3">
-        <v>-3</v>
-      </c>
       <c r="J20" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>162</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I21" s="3">
+        <v>-3</v>
+      </c>
       <c r="J21" t="s">
-        <v>130</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0.5</v>
+        <v>8</v>
       </c>
       <c r="J22" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>43</v>
       </c>
+      <c r="B23" t="s">
+        <v>162</v>
+      </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>141</v>
+        <v>37</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
       </c>
       <c r="H23" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I23" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J23" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="B24" t="s">
-        <v>162</v>
-      </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>8</v>
+        <v>141</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
       </c>
       <c r="I24" s="3">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>51</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>162</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I25" s="3">
+        <v>-5</v>
+      </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="3">
-        <v>-3</v>
-      </c>
       <c r="J26" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>162</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>122</v>
+        <v>38</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I27" s="3">
+        <v>-3</v>
+      </c>
       <c r="J27" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2107,68 +2172,68 @@
         <v>162</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="I29" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>162</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
       <c r="J30" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I31" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J31" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2179,68 +2244,68 @@
         <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="I32" s="3">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="J32" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>162</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="I33" s="3">
+        <v>-1</v>
+      </c>
       <c r="J33" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I34" s="3">
-        <v>0</v>
-      </c>
       <c r="J34" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2254,10 +2319,10 @@
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>8</v>
@@ -2266,7 +2331,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2280,48 +2345,54 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="3">
-        <v>23.5</v>
-      </c>
-      <c r="H36" s="3">
-        <v>40</v>
-      </c>
       <c r="I36" s="3">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>107</v>
-      </c>
-      <c r="K36" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>43</v>
       </c>
+      <c r="B37" t="s">
+        <v>162</v>
+      </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G37" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="H37" s="3">
+        <v>40</v>
+      </c>
+      <c r="I37" s="3">
+        <v>35</v>
+      </c>
       <c r="J37" t="s">
-        <v>45</v>
+        <v>107</v>
+      </c>
+      <c r="K37" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2332,39 +2403,36 @@
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J38" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J39" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2375,7 +2443,7 @@
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
         <v>74</v>
@@ -2384,7 +2452,7 @@
         <v>22</v>
       </c>
       <c r="I40" s="3">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="J40" t="s">
         <v>73</v>
@@ -2398,7 +2466,7 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
         <v>74</v>
@@ -2407,9 +2475,32 @@
         <v>22</v>
       </c>
       <c r="I41" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="3">
         <v>5</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
obsolete flux variables removed
</commit_message>
<xml_diff>
--- a/nitrogen_cycle_dynamics/nox_isotope_dynamics.xlsx
+++ b/nitrogen_cycle_dynamics/nox_isotope_dynamics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="22580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="162">
   <si>
     <t>id</t>
   </si>
@@ -239,9 +239,6 @@
     <t>\\delta^{18}O_{NO_{2}}</t>
   </si>
   <si>
-    <t>change</t>
-  </si>
-  <si>
     <t>c_Norg</t>
   </si>
   <si>
@@ -299,12 +296,6 @@
     <t>^{15}\\epsilon_{k,AAS}</t>
   </si>
   <si>
-    <t>\\Delta\[S\]</t>
-  </si>
-  <si>
-    <t>Change in substrate concentration</t>
-  </si>
-  <si>
     <t>c_NH4</t>
   </si>
   <si>
@@ -474,15 +465,6 @@
   </si>
   <si>
     <t>i\\delta^{15}N_{NO_{3}}</t>
-  </si>
-  <si>
-    <t>D1_conc</t>
-  </si>
-  <si>
-    <t>D2_conc</t>
-  </si>
-  <si>
-    <t>D3_conc</t>
   </si>
   <si>
     <t>\\left[NO_{3}\\right]</t>
@@ -1332,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1354,7 +1336,7 @@
         <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
@@ -1386,28 +1368,28 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1415,7 +1397,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1450,7 +1432,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -1482,16 +1464,16 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
         <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
@@ -1506,7 +1488,7 @@
         <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1514,16 +1496,16 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>8</v>
@@ -1538,10 +1520,10 @@
         <v>-13</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1549,16 +1531,16 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -1573,10 +1555,10 @@
         <v>-5</v>
       </c>
       <c r="J7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1584,16 +1566,16 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>8</v>
@@ -1608,10 +1590,10 @@
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1619,16 +1601,16 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>8</v>
@@ -1643,7 +1625,7 @@
         <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1651,16 +1633,16 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
@@ -1675,7 +1657,7 @@
         <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1683,16 +1665,16 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>8</v>
@@ -1707,7 +1689,7 @@
         <v>25</v>
       </c>
       <c r="J11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1715,16 +1697,16 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G12" s="3">
         <v>0.01</v>
@@ -1736,7 +1718,7 @@
         <v>0.2</v>
       </c>
       <c r="J12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1744,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1779,16 +1761,16 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>8</v>
@@ -1803,10 +1785,10 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1814,16 +1796,16 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
         <v>70</v>
-      </c>
-      <c r="E15" t="s">
-        <v>71</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>8</v>
@@ -1838,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1846,16 +1828,16 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>8</v>
@@ -1864,10 +1846,10 @@
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1875,7 +1857,7 @@
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1899,7 +1881,7 @@
         <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1910,7 +1892,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -1922,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1930,7 +1912,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1953,22 +1935,22 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1976,7 +1958,7 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1999,22 +1981,22 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2022,7 +2004,7 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -2046,7 +2028,7 @@
         <v>0.5</v>
       </c>
       <c r="J23" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2057,10 +2039,10 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
@@ -2069,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2077,7 +2059,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -2100,22 +2082,22 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2123,7 +2105,7 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -2146,22 +2128,22 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2169,25 +2151,25 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I29" s="3">
         <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2195,16 +2177,16 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>8</v>
@@ -2213,27 +2195,27 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2241,25 +2223,25 @@
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I32" s="3">
         <v>4</v>
       </c>
       <c r="J32" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2267,16 +2249,16 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>8</v>
@@ -2285,27 +2267,27 @@
         <v>-1</v>
       </c>
       <c r="J33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E34" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J34" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2313,16 +2295,16 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" t="s">
         <v>60</v>
-      </c>
-      <c r="E35" t="s">
-        <v>61</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>8</v>
@@ -2331,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2339,16 +2321,16 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>8</v>
@@ -2357,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2365,16 +2347,16 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>8</v>
@@ -2389,10 +2371,10 @@
         <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2433,75 +2415,6 @@
       </c>
       <c r="J39" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="3">
-        <v>10</v>
-      </c>
-      <c r="J40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" t="s">
-        <v>74</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" s="3">
-        <v>5</v>
-      </c>
-      <c r="J42" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2521,7 +2434,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2535,71 +2448,71 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>